<commit_message>
rule execution is working fine
</commit_message>
<xml_diff>
--- a/src/main/resources/rules.xlsx
+++ b/src/main/resources/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78E47BE-E220-477D-AE64-13129C3304F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF3653B-6484-41CE-A8EA-489615211D68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>RULE</t>
   </si>
@@ -48,10 +48,7 @@
 2. Check the general connection to the Active Directory.</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>java.net.ConnectException: Connection timed out: connect</t>
+    <t>java.net.ConnectException: Connection timed out: connect 8888</t>
   </si>
 </sst>
 </file>
@@ -406,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,15 +432,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
message includes exceptions also
</commit_message>
<xml_diff>
--- a/src/main/resources/rules.xlsx
+++ b/src/main/resources/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF3653B-6484-41CE-A8EA-489615211D68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9847E172-4A47-4E50-BD92-3CFD3F3681A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>RULE</t>
   </si>
@@ -48,7 +48,16 @@
 2. Check the general connection to the Active Directory.</t>
   </si>
   <si>
-    <t>java.net.ConnectException: Connection timed out: connect 8888</t>
+    <t>java.net.ConnectException: Connection timed out: connect</t>
+  </si>
+  <si>
+    <t>com.automationanywhere.token.exception.SecurityTokenMissingException: UM1117.access.token.not.found</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>1.Ask Client to clear all cache from browser and try to login again.</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +447,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rules are working by matching the hashset contains subset
</commit_message>
<xml_diff>
--- a/src/main/resources/rules.xlsx
+++ b/src/main/resources/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9847E172-4A47-4E50-BD92-3CFD3F3681A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A81A5-E5D4-49A3-9DA3-D9825B8A1167}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -44,20 +44,19 @@
     <t>R1</t>
   </si>
   <si>
-    <t>1. Check if Active Directory connection is working.
-2. Check the general connection to the Active Directory.</t>
-  </si>
-  <si>
-    <t>java.net.ConnectException: Connection timed out: connect</t>
-  </si>
-  <si>
-    <t>com.automationanywhere.token.exception.SecurityTokenMissingException: UM1117.access.token.not.found</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>1.Ask Client to clear all cache from browser and try to login again.</t>
+    <t>[LDAP: error code 49 - 80090308: LdapErr: DSID-0C09042F, comment: AcceptSecurityContext error, data 531, v2580 ]</t>
+  </si>
+  <si>
+    <t>Security token is invalid. java.util.NoSuchElementException: No value present</t>
+  </si>
+  <si>
+    <t>1. Ask client for Security token .</t>
+  </si>
+  <si>
+    <t>1. Ask client for microsoft error debugging.</t>
   </si>
 </sst>
 </file>
@@ -415,7 +414,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,18 +443,18 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logs and Rules file can be read directly from same jar folder
</commit_message>
<xml_diff>
--- a/src/main/resources/rules.xlsx
+++ b/src/main/resources/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A81A5-E5D4-49A3-9DA3-D9825B8A1167}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36A6774-65AC-4A8E-B1BD-F70921661218}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -53,10 +53,12 @@
     <t>Security token is invalid. java.util.NoSuchElementException: No value present</t>
   </si>
   <si>
-    <t>1. Ask client for Security token .</t>
-  </si>
-  <si>
-    <t>1. Ask client for microsoft error debugging.</t>
+    <t>Solution1:
+1. Ask client for microsoft error debugging.</t>
+  </si>
+  <si>
+    <t>Solution2:
+1. Ask client for Security token .</t>
   </si>
 </sst>
 </file>
@@ -414,7 +416,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +445,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -454,7 +456,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>